<commit_message>
Agregada ayudita al excel
</commit_message>
<xml_diff>
--- a/docs/plan-de-proyecto/anexos/flujo-cmh.xlsx
+++ b/docs/plan-de-proyecto/anexos/flujo-cmh.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="37200" windowHeight="21140" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="inversion inicial" sheetId="7" r:id="rId1"/>
@@ -255,7 +255,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -340,6 +340,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -375,7 +386,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -451,6 +462,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="32">
     <cellStyle name="Currency [0]" xfId="1" builtinId="7"/>
@@ -762,7 +776,7 @@
   <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView zoomScale="163" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -855,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="75" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="M45" sqref="L43:M45"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="75" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1422,7 +1436,10 @@
       <c r="E18" s="21"/>
       <c r="F18" s="21"/>
       <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
+      <c r="H18" s="21">
+        <f>SUM(H3:H17)</f>
+        <v>51760</v>
+      </c>
       <c r="I18" s="23">
         <f>SUM(I3:I17)</f>
         <v>3158333.3333333335</v>
@@ -1430,6 +1447,10 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="8"/>
+      <c r="H19" s="39">
+        <f>H18/60</f>
+        <v>862.66666666666663</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
@@ -2023,7 +2044,10 @@
       <c r="E40" s="21"/>
       <c r="F40" s="21"/>
       <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
+      <c r="H40" s="21">
+        <f>SUM(H25:H39)</f>
+        <v>6293.3333333333339</v>
+      </c>
       <c r="I40" s="23">
         <f>SUM(I25:I39)</f>
         <v>449444.44444444444</v>
@@ -2037,7 +2061,10 @@
       <c r="E41" s="13"/>
       <c r="F41" s="13"/>
       <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
+      <c r="H41" s="13">
+        <f>H40/60</f>
+        <v>104.8888888888889</v>
+      </c>
       <c r="I41" s="13"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -2048,7 +2075,10 @@
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
-      <c r="H42" s="16"/>
+      <c r="H42" s="16">
+        <f>H19-H41</f>
+        <v>757.77777777777771</v>
+      </c>
       <c r="I42" s="24"/>
     </row>
     <row r="43" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -2164,8 +2194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>